<commit_message>
Revert "Merge branch 'master' of https://github.com/KaasKop97/Project-3-Data"
This reverts commit c6bba72df54b131daa9bd2872e5eb49c7b738c98, reversing
changes made to b84c1b6943046ae496a67ec1c4dc06525bf3f547.
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Product backlog_Sprint 1,2,3,4 databases.xlsx
+++ b/Documents/Scrum/Product backlog_Sprint 1,2,3,4 databases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CI\Documents\School stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CI\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>product backlog</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Priority</t>
   </si>
   <si>
+    <t>H</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
@@ -50,12 +53,180 @@
     <t>User story</t>
   </si>
   <si>
+    <t>Time estimation</t>
+  </si>
+  <si>
     <t>Tasks</t>
   </si>
   <si>
     <t>Acceptance criteria</t>
   </si>
   <si>
+    <t>5 hours</t>
+  </si>
+  <si>
+    <t>As a user, i want a Create  a score screen so i know  how my game progression went.</t>
+  </si>
+  <si>
+    <t>As a user, I want a menu screen , so i have an option to exit the game.</t>
+  </si>
+  <si>
+    <t>As a Developer i want a prototype of the game obstacles  so i can challenge the players progress</t>
+  </si>
+  <si>
+    <t>10 hours</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Select the right screen size for menu
+• Lookup theories surounding screen design.
+• Test menu function for problems .
+• Write menu size in pygame
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Screen must not interfere with the games display 
+• Collected data can be applied to game
+• tests should be succesfull and function need to work
+• Test canvas is a succes
+• Code doesnt cause problems with other game functions
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Select the right screen size for score screen
+• Lookup theories surounding score screen design.
+• Test score screen function for problems .
+• Write score functions  in pygame
+</t>
+  </si>
+  <si>
+    <t>As a developer i want a prototype of the game pause menu so i can halt the game if needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Select the right screen size for pause screen
+• Lookup theories surounding pause screen design.
+• Test pause screen function for problems .
+• Write pause functions  in pygame
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Screen must  interfere with the games display 
+• Collected data can be applied to game
+• tests should be succesfull and function need to work
+• Pause has to stop the game temporarily but not score
+• Code doesnt cause problems with other game functions such as progression 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• search for theories surrounding game obstacles
+• studie obstacle behaviour with sprites
+• studie how obstacles effect the other code functions
+• Concept code for obstacles
+• make a base system file with obstacles 
+• test obstacles 
+• Rewrite code to support </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•theories can be applied to my game
+• studies support my sprites and basic function for obstacle works
+• Rewritten code  supports obstacles 
+• import file function works for obstacle file
+• Basic Character movements work  
+</t>
+  </si>
+  <si>
+    <t>As a developer i want a  pause menu so i can halt the game if needed.</t>
+  </si>
+  <si>
+    <t>As a player i want i visually stunning character so i can be represented as a gamecharacter.</t>
+  </si>
+  <si>
+    <t>As a user, i want visually stunning background graphics so i can enjoy the artstyle of the games.</t>
+  </si>
+  <si>
+    <t>20 hours</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>40 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• search for backgrounds that fit the theme of the game
+• studie obstacle behaviour with sprites
+• studie how obstacles effect the other code functions
+• Concept code for obstacles
+• Add background image to the sprites file
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• background must not interfere with the games display 
+• Collected data can be applied to game
+• tests should be succesfull and function of background need to work
+• Test game with new background should be flawless
+• Code of background doesnt cause problems with other game functions
+</t>
+  </si>
+  <si>
+    <t>• search for sprite based images for character
+• studie obstacle behaviour with sprites
+• resize character to fit the game
+• make a map and add character image in it
+• test character 
+• Rewrite code to support character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•character is the right size and fits inside the screen
+• character matches the theme of the game 
+• import image file works properly
+• Basic Character looks visually stunning
+</t>
+  </si>
+  <si>
+    <t>• search for bugs in the code and look what causes them
+• studie obstacle behaviour with sprites
+• studie how obstacles effect the other code functions and fix errors
+• test new code 
+• Rewrite code to support the extra lines of code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• bugs surrounding code are fixed
+• test code is successfull
+• studie how obstacles effect the other code functions
+• test of new code is successfull and works properly 
+</t>
+  </si>
+  <si>
+    <t>• search for bugs in the code and look what causes all games to not load
+• studie videos surrounding adding mutiple types of code to one file
+• studie how obstacles effect the other code functions and fix errors
+• Rewrite code to support all games at the same time</t>
+  </si>
+  <si>
+    <t>• search for bugs in the code and look what causes all games to not load can be applied to our game menue
+• Rewritten code to support all games at the same time works</t>
+  </si>
+  <si>
+    <t>• Search for music that fits the team of the game
+• Add sound fuction to the game settings file</t>
+  </si>
+  <si>
+    <t>• Ambient noice volume is mild and not distracting to the player
+• Add sound fuction plays music when game starts</t>
+  </si>
+  <si>
+    <t>As a developer i want bugs fixed so the player can enjoy the game.</t>
+  </si>
+  <si>
+    <t>As a player i want one game menu ,so i can  access all the minigames from one place.</t>
+  </si>
+  <si>
+    <t>As a player i want ambient noise , i can enjoy the game sounds while playing the game in peace.</t>
+  </si>
+  <si>
     <t>The app has to receive data from datasets</t>
   </si>
   <si>
@@ -111,6 +282,12 @@
   </si>
   <si>
     <t>As a developer i want a programming language so i can write code that receives data from collected datasets.</t>
+  </si>
+  <si>
+    <t>0.5 hours</t>
+  </si>
+  <si>
+    <t>1 hour</t>
   </si>
   <si>
     <t xml:space="preserve">• Brainstorm on what aspect ratio will work best for the app.
@@ -163,278 +340,6 @@
     <t>• Discuss with team if datasets can be used.
 • Look up information surrounding datasets . 
 • Add datasets to file collection for later use.</t>
-  </si>
-  <si>
-    <t>As a user i want a variation of tables on the webpage so i can view the data i want to see based on the filters i selected.</t>
-  </si>
-  <si>
-    <t>As a user i want a help button that brings me to a help screen so i can see the developers contact information , information about the website and database .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Select the right screen size for  app screen.
-• Lookup theories surounding score screen design.
-• use  test color schemes to find right ui for app.
-</t>
-  </si>
-  <si>
-    <t>As a Developer i want a program to write code in so i can add visual graphics to the webpage upon which user will be able to view data in tables on.</t>
-  </si>
-  <si>
-    <t>download C# , Visualstudio , Ryder
-• Concept code for webpage
-• Rewrite code to support elements on webpage</t>
-  </si>
-  <si>
-    <t>As a user i want a working sub app window so i can look  up de data i want to see.</t>
-  </si>
-  <si>
-    <t>As i user i want various buttons so i can navigate through the app window.</t>
-  </si>
-  <si>
-    <t>As a developer i want a set of queries to derive information from the database.</t>
-  </si>
-  <si>
-    <t>As a user i want a color scheme that doesnt interfere with the navigation and the text on the screen so i can differentiate between ui elements.</t>
-  </si>
-  <si>
-    <t>Storypoints</t>
-  </si>
-  <si>
-    <t>30 points</t>
-  </si>
-  <si>
-    <t>20 points</t>
-  </si>
-  <si>
-    <t>10 points</t>
-  </si>
-  <si>
-    <t>5 points</t>
-  </si>
-  <si>
-    <t>1 point</t>
-  </si>
-  <si>
-    <t>4 points</t>
-  </si>
-  <si>
-    <t>3 points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 points    </t>
-  </si>
-  <si>
-    <t>As a user i want a  graph of the questions i want answerd so i can derive my answer from the graph.</t>
-  </si>
-  <si>
-    <t>15 points</t>
-  </si>
-  <si>
-    <t>As a developer i want a working database so i can derive information from the tables to answer my queries.</t>
-  </si>
-  <si>
-    <t>As a developer i want a working website interface so i can test the grahpics of the diagrams on.</t>
-  </si>
-  <si>
-    <t>As a user i want a storyboard translated into a digital mockup how the website is going to behave so i know how to navigate through the pages of the webapplication.</t>
-  </si>
-  <si>
-    <t>As a developer i want to translate my sub-questions into postgresql queries so i can derive information and put that information into tables for the users to view.</t>
-  </si>
-  <si>
-    <t>As a user i want a home button so i can return to the homepage upon which i started.</t>
-  </si>
-  <si>
-    <t>As a user i want a escape button so i can exit the webpage if needed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a developer i want graphs best representing the  subquestions so  the user can have good overview of what the answers are to those questions . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Create an erd model.
-• Lookup data in data sets.
-• Test data base for value inputs and relationships.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Brainstorm on what aspect ratio will work best for the app.
-• Sketch UI elements  are translated into digital model.
-• Test the page navigation .
-</t>
-  </si>
-  <si>
-    <t>• Translate erd  relationships and connections  into queries for  database language.
-• Add values from datasets into tables.
-• Call apon values for testing.</t>
-  </si>
-  <si>
-    <t>• Create tables for the website in visualstudio.
-• Add values of queries into the tables.
-• Create basic filters for testing.</t>
-  </si>
-  <si>
-    <t>• Brainstorm where to put home button.
-• Write code for working home button.
-• Test position of home button with test users.</t>
-  </si>
-  <si>
-    <t>• Brainstorm where to put help button    .                                     • Brainstorm what information will be displayed when pressed.
-• Write code for working help button.
-• Test position of help button with test users.</t>
-  </si>
-  <si>
-    <t>• Brainstorm where to put escape button .                               
-• Write code for working escape button.
-• Test position of escape button with test users.</t>
-  </si>
-  <si>
-    <t>• Brainstorm about which graphs best fit the data that needs to be viewed.                                                                                         • Brainstorm what information will be displayed when selected.
-• Choose what the y-axis looks like and the x-axis looks like.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• The data is best represented by a particular graph.
-•The axes have the right information on them   .                            </t>
-  </si>
-  <si>
-    <t>• Escape button should close all pages from app .                                           
-• Escape button should be visible at first glance.</t>
-  </si>
-  <si>
-    <t>• Help button should be visible at first glance.
-• Collected data from test can be used for improving help button fuction if needed.
-• Help brings user to information screen about webpage.
-• Code doesnt cause problems with other page elements.</t>
-  </si>
-  <si>
-    <t>• Home button should be visible at first glance.
-• Collected data from test can be used for improving home  button fuction if needed.
-• Homebutton brings user to start screen.
-• Code doesnt cause problems with other page elements.</t>
-  </si>
-  <si>
-    <t>•Tables have data asked by user and are loaded on page.
-• Values have enough information to answer user question.
-• Filters add variation in data displayed.</t>
-  </si>
-  <si>
-    <t>• Erd  relationships and connections work in database language.
-• Collected data can be called in the database.
-• Tables work and have enough data for visualization.
-• Queries dont cause problems in other tables.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">•All programs are setup and working.
-• Rewritten code  has no errors. 
-• Basic navigation works.  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Screen must not interfere with the  display of page elements.
-• User can navigation  without to much clicking of mouse.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Screen must not interfere with app ui elements.
-• Collected data can be applied to page.
-• tests should be succesfull and function need to work.
-• Test canvas has matching color and is readable. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Erd must show relationships and connections.
-• Collected data can be applied to database.
-• Tests should be succesfull and functions need to work.
-• Code doesnt cause problems with other sets.
-</t>
-  </si>
-  <si>
-    <t>As a user i want  filters on the app so i can filter out the data i want to vizualise .</t>
-  </si>
-  <si>
-    <t>As a user i want  a bug free app so i can smoothly use the app.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-•Write code to create app window.
-•Test menu function with test group .
-•Write code in plugin to make ui element work.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Write queries that will act as filters on the database.
-• Decide what data needs to be vizualized from database.
-• write code that adds filters to the app window.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Write working queries .
-</t>
-  </si>
-  <si>
-    <t>• Choose a set of colors for the app ui.
-•Design the ui in wordform .
-• Edit elements to not interfere with eachother.
-•Test color scheme on users groups using the app .</t>
-  </si>
-  <si>
-    <t>• Fix ui errors if needed.
-•Fix design errors if needed.
-• Fix bugs in the code .
-•Test color scheme on users groups using the app .</t>
-  </si>
-  <si>
-    <t>• Ui errors have all been fixed.
-• Design errors have all been fixed.
-• Bugs in code have all been fixed.
-•Test color scheme  is accepted by many users.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• The text on the screen needs to be readable to users.
-• Ui elements need a basic form so it is recognizable to any user.
-• Edited ui elements dont interfere with eachother in anyway.
-•Test color scheme is to the user liking and not  to busy.
-</t>
-  </si>
-  <si>
-    <t>• All buttons should be visible at first glance to users.
-• Code doesnt cause problems with other page elements.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Qeuries are able to pull data out of more than 2 columns and more than 2 tables and perform certain mathematic tasks needed for some of the graphs.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Graph has y and x-axis that use the right columns.
-• Optional Graph can also provide the reight columns per axis but has a different vizualisation style.
-• Values are pulled from the the data base created by team.
-• Pause has to stop the game temporarily but not score.
-• Most user must be able to understand the info in the graphs.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Queries can derive less data or more data depending on what filter is selected.
-• The data derived from tha database will provide enough information to answer the new filterd question.
-• Code of the filters doesnt cause problems with other app  functions.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Code doesnt cause problems with main menu.
-•  Test group can use the windows without happering .
-• tests should be succesfull and function need to work.
-• Code doesnt cause problems with  the main app and other app windows of subgroups 2 and 1.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Select the right graph to represent the data.
-•Select other optional graph types in case main graph doesnt provide enough information to user.
-• Insert values into graph to draw graph.
-•Test graph with users to see if the info is understandable .
-</t>
-  </si>
-  <si>
-    <t>• Choose final button positions    .                                                      
-• Edit written code for working  buttons in plugin.
-• Test position of buttons with test users.</t>
   </si>
 </sst>
 </file>
@@ -553,7 +458,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
@@ -575,7 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
@@ -936,10 +840,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,10 +851,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,10 +862,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -969,10 +873,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -980,10 +884,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,10 +895,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,10 +906,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,10 +928,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1035,10 +939,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,10 +950,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1075,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="4"/>
@@ -1200,19 +1104,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>47</v>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1220,19 +1124,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1240,19 +1144,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1260,19 +1164,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1280,19 +1184,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1300,19 +1204,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1323,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="4"/>
@@ -1369,201 +1273,99 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>47</v>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1576,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1393,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="4"/>
@@ -1620,19 +1422,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>47</v>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1640,136 +1442,139 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/KaasKop97/Project-3-Data""
This reverts commit 01e9a4eec1bf7485ba0afc43da1972c26478bcbf.
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Product backlog_Sprint 1,2,3,4 databases.xlsx
+++ b/Documents/Scrum/Product backlog_Sprint 1,2,3,4 databases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CI\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CI\Documents\School stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="99">
   <si>
     <t>product backlog</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -53,180 +50,12 @@
     <t>User story</t>
   </si>
   <si>
-    <t>Time estimation</t>
-  </si>
-  <si>
     <t>Tasks</t>
   </si>
   <si>
     <t>Acceptance criteria</t>
   </si>
   <si>
-    <t>5 hours</t>
-  </si>
-  <si>
-    <t>As a user, i want a Create  a score screen so i know  how my game progression went.</t>
-  </si>
-  <si>
-    <t>As a user, I want a menu screen , so i have an option to exit the game.</t>
-  </si>
-  <si>
-    <t>As a Developer i want a prototype of the game obstacles  so i can challenge the players progress</t>
-  </si>
-  <si>
-    <t>10 hours</t>
-  </si>
-  <si>
-    <t>3 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Select the right screen size for menu
-• Lookup theories surounding screen design.
-• Test menu function for problems .
-• Write menu size in pygame
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Screen must not interfere with the games display 
-• Collected data can be applied to game
-• tests should be succesfull and function need to work
-• Test canvas is a succes
-• Code doesnt cause problems with other game functions
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Select the right screen size for score screen
-• Lookup theories surounding score screen design.
-• Test score screen function for problems .
-• Write score functions  in pygame
-</t>
-  </si>
-  <si>
-    <t>As a developer i want a prototype of the game pause menu so i can halt the game if needed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Select the right screen size for pause screen
-• Lookup theories surounding pause screen design.
-• Test pause screen function for problems .
-• Write pause functions  in pygame
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Screen must  interfere with the games display 
-• Collected data can be applied to game
-• tests should be succesfull and function need to work
-• Pause has to stop the game temporarily but not score
-• Code doesnt cause problems with other game functions such as progression 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• search for theories surrounding game obstacles
-• studie obstacle behaviour with sprites
-• studie how obstacles effect the other code functions
-• Concept code for obstacles
-• make a base system file with obstacles 
-• test obstacles 
-• Rewrite code to support </t>
-  </si>
-  <si>
-    <t xml:space="preserve">•theories can be applied to my game
-• studies support my sprites and basic function for obstacle works
-• Rewritten code  supports obstacles 
-• import file function works for obstacle file
-• Basic Character movements work  
-</t>
-  </si>
-  <si>
-    <t>As a developer i want a  pause menu so i can halt the game if needed.</t>
-  </si>
-  <si>
-    <t>As a player i want i visually stunning character so i can be represented as a gamecharacter.</t>
-  </si>
-  <si>
-    <t>As a user, i want visually stunning background graphics so i can enjoy the artstyle of the games.</t>
-  </si>
-  <si>
-    <t>20 hours</t>
-  </si>
-  <si>
-    <t>2 hours</t>
-  </si>
-  <si>
-    <t>40 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• search for backgrounds that fit the theme of the game
-• studie obstacle behaviour with sprites
-• studie how obstacles effect the other code functions
-• Concept code for obstacles
-• Add background image to the sprites file
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• background must not interfere with the games display 
-• Collected data can be applied to game
-• tests should be succesfull and function of background need to work
-• Test game with new background should be flawless
-• Code of background doesnt cause problems with other game functions
-</t>
-  </si>
-  <si>
-    <t>• search for sprite based images for character
-• studie obstacle behaviour with sprites
-• resize character to fit the game
-• make a map and add character image in it
-• test character 
-• Rewrite code to support character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">•character is the right size and fits inside the screen
-• character matches the theme of the game 
-• import image file works properly
-• Basic Character looks visually stunning
-</t>
-  </si>
-  <si>
-    <t>• search for bugs in the code and look what causes them
-• studie obstacle behaviour with sprites
-• studie how obstacles effect the other code functions and fix errors
-• test new code 
-• Rewrite code to support the extra lines of code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• bugs surrounding code are fixed
-• test code is successfull
-• studie how obstacles effect the other code functions
-• test of new code is successfull and works properly 
-</t>
-  </si>
-  <si>
-    <t>• search for bugs in the code and look what causes all games to not load
-• studie videos surrounding adding mutiple types of code to one file
-• studie how obstacles effect the other code functions and fix errors
-• Rewrite code to support all games at the same time</t>
-  </si>
-  <si>
-    <t>• search for bugs in the code and look what causes all games to not load can be applied to our game menue
-• Rewritten code to support all games at the same time works</t>
-  </si>
-  <si>
-    <t>• Search for music that fits the team of the game
-• Add sound fuction to the game settings file</t>
-  </si>
-  <si>
-    <t>• Ambient noice volume is mild and not distracting to the player
-• Add sound fuction plays music when game starts</t>
-  </si>
-  <si>
-    <t>As a developer i want bugs fixed so the player can enjoy the game.</t>
-  </si>
-  <si>
-    <t>As a player i want one game menu ,so i can  access all the minigames from one place.</t>
-  </si>
-  <si>
-    <t>As a player i want ambient noise , i can enjoy the game sounds while playing the game in peace.</t>
-  </si>
-  <si>
     <t>The app has to receive data from datasets</t>
   </si>
   <si>
@@ -282,12 +111,6 @@
   </si>
   <si>
     <t>As a developer i want a programming language so i can write code that receives data from collected datasets.</t>
-  </si>
-  <si>
-    <t>0.5 hours</t>
-  </si>
-  <si>
-    <t>1 hour</t>
   </si>
   <si>
     <t xml:space="preserve">• Brainstorm on what aspect ratio will work best for the app.
@@ -340,6 +163,278 @@
     <t>• Discuss with team if datasets can be used.
 • Look up information surrounding datasets . 
 • Add datasets to file collection for later use.</t>
+  </si>
+  <si>
+    <t>As a user i want a variation of tables on the webpage so i can view the data i want to see based on the filters i selected.</t>
+  </si>
+  <si>
+    <t>As a user i want a help button that brings me to a help screen so i can see the developers contact information , information about the website and database .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Select the right screen size for  app screen.
+• Lookup theories surounding score screen design.
+• use  test color schemes to find right ui for app.
+</t>
+  </si>
+  <si>
+    <t>As a Developer i want a program to write code in so i can add visual graphics to the webpage upon which user will be able to view data in tables on.</t>
+  </si>
+  <si>
+    <t>download C# , Visualstudio , Ryder
+• Concept code for webpage
+• Rewrite code to support elements on webpage</t>
+  </si>
+  <si>
+    <t>As a user i want a working sub app window so i can look  up de data i want to see.</t>
+  </si>
+  <si>
+    <t>As i user i want various buttons so i can navigate through the app window.</t>
+  </si>
+  <si>
+    <t>As a developer i want a set of queries to derive information from the database.</t>
+  </si>
+  <si>
+    <t>As a user i want a color scheme that doesnt interfere with the navigation and the text on the screen so i can differentiate between ui elements.</t>
+  </si>
+  <si>
+    <t>Storypoints</t>
+  </si>
+  <si>
+    <t>30 points</t>
+  </si>
+  <si>
+    <t>20 points</t>
+  </si>
+  <si>
+    <t>10 points</t>
+  </si>
+  <si>
+    <t>5 points</t>
+  </si>
+  <si>
+    <t>1 point</t>
+  </si>
+  <si>
+    <t>4 points</t>
+  </si>
+  <si>
+    <t>3 points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 points    </t>
+  </si>
+  <si>
+    <t>As a user i want a  graph of the questions i want answerd so i can derive my answer from the graph.</t>
+  </si>
+  <si>
+    <t>15 points</t>
+  </si>
+  <si>
+    <t>As a developer i want a working database so i can derive information from the tables to answer my queries.</t>
+  </si>
+  <si>
+    <t>As a developer i want a working website interface so i can test the grahpics of the diagrams on.</t>
+  </si>
+  <si>
+    <t>As a user i want a storyboard translated into a digital mockup how the website is going to behave so i know how to navigate through the pages of the webapplication.</t>
+  </si>
+  <si>
+    <t>As a developer i want to translate my sub-questions into postgresql queries so i can derive information and put that information into tables for the users to view.</t>
+  </si>
+  <si>
+    <t>As a user i want a home button so i can return to the homepage upon which i started.</t>
+  </si>
+  <si>
+    <t>As a user i want a escape button so i can exit the webpage if needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a developer i want graphs best representing the  subquestions so  the user can have good overview of what the answers are to those questions . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Create an erd model.
+• Lookup data in data sets.
+• Test data base for value inputs and relationships.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Brainstorm on what aspect ratio will work best for the app.
+• Sketch UI elements  are translated into digital model.
+• Test the page navigation .
+</t>
+  </si>
+  <si>
+    <t>• Translate erd  relationships and connections  into queries for  database language.
+• Add values from datasets into tables.
+• Call apon values for testing.</t>
+  </si>
+  <si>
+    <t>• Create tables for the website in visualstudio.
+• Add values of queries into the tables.
+• Create basic filters for testing.</t>
+  </si>
+  <si>
+    <t>• Brainstorm where to put home button.
+• Write code for working home button.
+• Test position of home button with test users.</t>
+  </si>
+  <si>
+    <t>• Brainstorm where to put help button    .                                     • Brainstorm what information will be displayed when pressed.
+• Write code for working help button.
+• Test position of help button with test users.</t>
+  </si>
+  <si>
+    <t>• Brainstorm where to put escape button .                               
+• Write code for working escape button.
+• Test position of escape button with test users.</t>
+  </si>
+  <si>
+    <t>• Brainstorm about which graphs best fit the data that needs to be viewed.                                                                                         • Brainstorm what information will be displayed when selected.
+• Choose what the y-axis looks like and the x-axis looks like.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• The data is best represented by a particular graph.
+•The axes have the right information on them   .                            </t>
+  </si>
+  <si>
+    <t>• Escape button should close all pages from app .                                           
+• Escape button should be visible at first glance.</t>
+  </si>
+  <si>
+    <t>• Help button should be visible at first glance.
+• Collected data from test can be used for improving help button fuction if needed.
+• Help brings user to information screen about webpage.
+• Code doesnt cause problems with other page elements.</t>
+  </si>
+  <si>
+    <t>• Home button should be visible at first glance.
+• Collected data from test can be used for improving home  button fuction if needed.
+• Homebutton brings user to start screen.
+• Code doesnt cause problems with other page elements.</t>
+  </si>
+  <si>
+    <t>•Tables have data asked by user and are loaded on page.
+• Values have enough information to answer user question.
+• Filters add variation in data displayed.</t>
+  </si>
+  <si>
+    <t>• Erd  relationships and connections work in database language.
+• Collected data can be called in the database.
+• Tables work and have enough data for visualization.
+• Queries dont cause problems in other tables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•All programs are setup and working.
+• Rewritten code  has no errors. 
+• Basic navigation works.  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Screen must not interfere with the  display of page elements.
+• User can navigation  without to much clicking of mouse.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Screen must not interfere with app ui elements.
+• Collected data can be applied to page.
+• tests should be succesfull and function need to work.
+• Test canvas has matching color and is readable. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Erd must show relationships and connections.
+• Collected data can be applied to database.
+• Tests should be succesfull and functions need to work.
+• Code doesnt cause problems with other sets.
+</t>
+  </si>
+  <si>
+    <t>As a user i want  filters on the app so i can filter out the data i want to vizualise .</t>
+  </si>
+  <si>
+    <t>As a user i want  a bug free app so i can smoothly use the app.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+•Write code to create app window.
+•Test menu function with test group .
+•Write code in plugin to make ui element work.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Write queries that will act as filters on the database.
+• Decide what data needs to be vizualized from database.
+• write code that adds filters to the app window.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Write working queries .
+</t>
+  </si>
+  <si>
+    <t>• Choose a set of colors for the app ui.
+•Design the ui in wordform .
+• Edit elements to not interfere with eachother.
+•Test color scheme on users groups using the app .</t>
+  </si>
+  <si>
+    <t>• Fix ui errors if needed.
+•Fix design errors if needed.
+• Fix bugs in the code .
+•Test color scheme on users groups using the app .</t>
+  </si>
+  <si>
+    <t>• Ui errors have all been fixed.
+• Design errors have all been fixed.
+• Bugs in code have all been fixed.
+•Test color scheme  is accepted by many users.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• The text on the screen needs to be readable to users.
+• Ui elements need a basic form so it is recognizable to any user.
+• Edited ui elements dont interfere with eachother in anyway.
+•Test color scheme is to the user liking and not  to busy.
+</t>
+  </si>
+  <si>
+    <t>• All buttons should be visible at first glance to users.
+• Code doesnt cause problems with other page elements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Qeuries are able to pull data out of more than 2 columns and more than 2 tables and perform certain mathematic tasks needed for some of the graphs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Graph has y and x-axis that use the right columns.
+• Optional Graph can also provide the reight columns per axis but has a different vizualisation style.
+• Values are pulled from the the data base created by team.
+• Pause has to stop the game temporarily but not score.
+• Most user must be able to understand the info in the graphs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Queries can derive less data or more data depending on what filter is selected.
+• The data derived from tha database will provide enough information to answer the new filterd question.
+• Code of the filters doesnt cause problems with other app  functions.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Code doesnt cause problems with main menu.
+•  Test group can use the windows without happering .
+• tests should be succesfull and function need to work.
+• Code doesnt cause problems with  the main app and other app windows of subgroups 2 and 1.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Select the right graph to represent the data.
+•Select other optional graph types in case main graph doesnt provide enough information to user.
+• Insert values into graph to draw graph.
+•Test graph with users to see if the info is understandable .
+</t>
+  </si>
+  <si>
+    <t>• Choose final button positions    .                                                      
+• Edit written code for working  buttons in plugin.
+• Test position of buttons with test users.</t>
   </si>
 </sst>
 </file>
@@ -458,7 +553,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
@@ -480,6 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
@@ -840,10 +936,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -851,10 +947,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,10 +958,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -873,10 +969,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,10 +980,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,10 +991,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,10 +1002,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,10 +1013,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,10 +1024,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,10 +1035,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,10 +1046,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1171,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="4"/>
@@ -1104,19 +1200,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1124,19 +1220,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1144,19 +1240,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1164,19 +1260,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1184,19 +1280,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1204,19 +1300,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1227,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,7 +1340,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="4"/>
@@ -1273,99 +1369,201 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>24</v>
+      <c r="D10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1378,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1591,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="4"/>
@@ -1422,19 +1620,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1442,139 +1640,136 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>